<commit_message>
EPBDS-8950 Customizing output of a SpreadsheetResult using `exclusion`. Tests.
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment4/simple4/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment4/simple4/module1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment4\simple4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F7941-9C17-4479-BB06-FBFE5C51BB8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90675377-D391-4BA4-83DA-32FA570C9336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1470" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="mysprs" sheetId="8" r:id="rId4"/>
     <sheet name="mysprs2" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -276,15 +276,9 @@
     <t>Spreadsheet SpreadsheetResult mySpr()</t>
   </si>
   <si>
-    <t>Value2</t>
-  </si>
-  <si>
     <t>Step2*</t>
   </si>
   <si>
-    <t>Value1*</t>
-  </si>
-  <si>
     <t>Step1*</t>
   </si>
   <si>
@@ -336,12 +330,6 @@
     <t>Step4*</t>
   </si>
   <si>
-    <t>Value3*</t>
-  </si>
-  <si>
-    <t>Value4*</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult mySpr2()</t>
   </si>
   <si>
@@ -409,6 +397,18 @@
   </si>
   <si>
     <t>detailedPlainModel</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Value4</t>
+  </si>
+  <si>
+    <t>Value2~</t>
+  </si>
+  <si>
+    <t>Value1</t>
   </si>
 </sst>
 </file>
@@ -806,24 +806,24 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -831,18 +831,18 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -852,7 +852,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -862,7 +862,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -872,7 +872,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -890,7 +890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -898,15 +898,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -914,7 +914,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -922,7 +922,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -930,24 +930,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -956,7 +956,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
@@ -964,7 +964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
@@ -972,40 +972,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>77</v>
       </c>
@@ -1013,34 +1013,34 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -1049,7 +1049,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1057,7 +1057,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1065,7 +1065,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>34</v>
@@ -1075,7 +1075,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>36</v>
@@ -1129,7 +1129,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -1183,7 +1183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>37</v>
@@ -1237,7 +1237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1245,7 +1245,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1253,13 +1253,13 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>2</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>10</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
         <v>19</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>21</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>57</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>23</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>25</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>28</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>62</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>63</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>64</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>65</v>
       </c>
@@ -1440,9 +1440,9 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1450,7 +1450,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1458,7 +1458,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1468,7 +1468,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1480,7 +1480,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -1492,7 +1492,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1504,7 +1504,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1516,7 +1516,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1528,7 +1528,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1540,19 +1540,19 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1576,25 +1576,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>25</v>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>28</v>
@@ -1624,47 +1624,47 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>77</v>
@@ -1674,43 +1674,43 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1729,15 +1729,15 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
     </row>
@@ -1767,18 +1767,18 @@
   <dimension ref="A2:E27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1786,67 +1786,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1855,9 +1855,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1866,42 +1866,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>35</v>
@@ -1911,22 +1911,22 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11">
@@ -1943,19 +1943,19 @@
   <dimension ref="B3:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1964,97 +1964,97 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -2063,9 +2063,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="11">
         <v>3</v>
@@ -2074,43 +2074,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>35</v>
@@ -2119,9 +2119,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2129,12 +2129,12 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="11">
         <v>1</v>

</xml_diff>